<commit_message>
updated notes through module 4
</commit_message>
<xml_diff>
--- a/Stat5100/course/F20 Schedule (Stat 5100).xlsx
+++ b/Stat5100/course/F20 Schedule (Stat 5100).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79AEEC6-6477-4C46-BC04-8ED88C883A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9275D962-F5C0-476E-835B-FA800D0676AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,21 +225,12 @@
     <t>Mid-Semester Eval</t>
   </si>
   <si>
-    <t>Model Interpretabillity</t>
-  </si>
-  <si>
-    <t>Group Work Primer</t>
-  </si>
-  <si>
     <t>HW 4/Project 1 Paper - Final Draft</t>
   </si>
   <si>
     <t>Mythos of Model Interpretability</t>
   </si>
   <si>
-    <t>Final Project Introductions</t>
-  </si>
-  <si>
     <t>Quiz 6 (Bonus Quiz - Free Extra Drop)</t>
   </si>
   <si>
@@ -249,10 +240,19 @@
     <t>Final Project Update</t>
   </si>
   <si>
-    <t>7.3: Modern Applications</t>
-  </si>
-  <si>
     <t>Final Project Slides (pdf format)</t>
+  </si>
+  <si>
+    <t>No Class (Interim Day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Work Primer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model Interpretabillity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Project Introductions </t>
   </si>
 </sst>
 </file>
@@ -387,11 +387,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,11 +687,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -933,7 +933,7 @@
         <v>38</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -963,10 +963,10 @@
         <v>44134</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -974,7 +974,7 @@
         <v>44137</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>26</v>
@@ -985,7 +985,7 @@
         <v>44139</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C31" s="11"/>
     </row>
@@ -1004,7 +1004,7 @@
       <c r="A33" s="4">
         <v>44144</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="5"/>
@@ -1068,7 +1068,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1117,7 +1117,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1139,18 +1139,18 @@
         <v>43</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>44176</v>
       </c>
-      <c r="B47" s="17" t="s">
-        <v>60</v>
+      <c r="B47" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1175,7 +1175,7 @@
       <c r="C50" s="12"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="23" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all notes updated except 7.1
</commit_message>
<xml_diff>
--- a/Stat5100/course/F20 Schedule (Stat 5100).xlsx
+++ b/Stat5100/course/F20 Schedule (Stat 5100).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9275D962-F5C0-476E-835B-FA800D0676AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6DB4FE-2B07-4A8E-B4CF-9EFCF30749BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>Quiz 5</t>
-  </si>
-  <si>
-    <t>Project 2 Peer Review/Final Project Proposals</t>
   </si>
   <si>
     <t>Review Response/Final Project Papers - Final Draft</t>
@@ -204,9 +201,6 @@
     <t>HW 5/Project 2 Papers - First Draft</t>
   </si>
   <si>
-    <t>HW 6/Project 2 Papers - Final Draft</t>
-  </si>
-  <si>
     <t>6.2 Time Series Case Study</t>
   </si>
   <si>
@@ -237,9 +231,6 @@
     <t xml:space="preserve">Final Project Papers - Penultimate Draft </t>
   </si>
   <si>
-    <t>Final Project Update</t>
-  </si>
-  <si>
     <t>Final Project Slides (pdf format)</t>
   </si>
   <si>
@@ -253,13 +244,41 @@
   </si>
   <si>
     <t xml:space="preserve">Final Project Introductions </t>
+  </si>
+  <si>
+    <t>(Applications and Examples - Homework 7)</t>
+  </si>
+  <si>
+    <t>Final Project Proposals</t>
+  </si>
+  <si>
+    <t>Project 2 Peer Review</t>
+  </si>
+  <si>
+    <t>HW 6</t>
+  </si>
+  <si>
+    <r>
+      <t>Final Project Update/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project 2 Papers - Final Draft</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +322,14 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -392,6 +419,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,7 +703,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,7 +737,7 @@
         <v>44074</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -738,7 +766,7 @@
         <v>44081</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -756,7 +784,7 @@
         <v>44085</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>5</v>
@@ -767,7 +795,7 @@
         <v>44088</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -785,7 +813,7 @@
         <v>44092</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="10"/>
     </row>
@@ -812,7 +840,7 @@
         <v>44099</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>4</v>
@@ -843,7 +871,7 @@
         <v>44106</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="10"/>
     </row>
@@ -870,7 +898,7 @@
         <v>44113</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>13</v>
@@ -890,7 +918,7 @@
         <v>44118</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>28</v>
@@ -901,7 +929,7 @@
         <v>44120</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>12</v>
@@ -921,7 +949,7 @@
         <v>44125</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="12"/>
     </row>
@@ -930,10 +958,10 @@
         <v>44127</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -941,10 +969,10 @@
         <v>44130</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -952,7 +980,7 @@
         <v>44132</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>29</v>
@@ -963,10 +991,10 @@
         <v>44134</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -974,7 +1002,7 @@
         <v>44137</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>26</v>
@@ -985,7 +1013,7 @@
         <v>44139</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" s="11"/>
     </row>
@@ -994,10 +1022,10 @@
         <v>44141</v>
       </c>
       <c r="B32" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1025,10 +1053,10 @@
         <v>44148</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1038,14 +1066,16 @@
       <c r="B36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="26" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44153</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C37" s="12"/>
     </row>
@@ -1054,10 +1084,10 @@
         <v>44155</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1065,10 +1095,10 @@
         <v>44158</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1076,7 +1106,7 @@
         <v>44160</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>31</v>
@@ -1087,7 +1117,7 @@
         <v>44162</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="10"/>
     </row>
@@ -1096,7 +1126,7 @@
         <v>44165</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="6"/>
     </row>
@@ -1105,7 +1135,7 @@
         <v>44167</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="3"/>
     </row>
@@ -1114,10 +1144,10 @@
         <v>44169</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1125,10 +1155,10 @@
         <v>44172</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1136,10 +1166,10 @@
         <v>44174</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1147,10 +1177,10 @@
         <v>44176</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1161,7 +1191,7 @@
         <v>24</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1176,7 +1206,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B52" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>